<commit_message>
creation diagramme de gantt
</commit_message>
<xml_diff>
--- a/Cahier des charges.xlsx
+++ b/Cahier des charges.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
   <si>
     <t>Fonctionnalités</t>
   </si>
@@ -246,13 +247,76 @@
   </si>
   <si>
     <t>modifier la liste des ingredient</t>
+  </si>
+  <si>
+    <t>bdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user </t>
+  </si>
+  <si>
+    <t>inscription /connexion etc</t>
+  </si>
+  <si>
+    <t>j'ai faim</t>
+  </si>
+  <si>
+    <t>Creation BDD</t>
+  </si>
+  <si>
+    <t>Partie User</t>
+  </si>
+  <si>
+    <t>Partie J'ai faim</t>
+  </si>
+  <si>
+    <t>Partie commentaire</t>
+  </si>
+  <si>
+    <t>Partie theme</t>
+  </si>
+  <si>
+    <t>Partie administration</t>
+  </si>
+  <si>
+    <t>Fonction Favoris</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Theo</t>
+  </si>
+  <si>
+    <t>Sammy</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>HTML partie client</t>
+  </si>
+  <si>
+    <t>HTML parte administration</t>
+  </si>
+  <si>
+    <t>Design/CSS</t>
+  </si>
+  <si>
+    <t>Requete AJAX j'ai faim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,16 +354,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -485,11 +587,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -510,15 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -532,6 +653,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,39 +957,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
       <c r="H2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
       <c r="P2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>19</v>
@@ -862,7 +1007,7 @@
       <c r="N3" s="6"/>
       <c r="P3" s="15"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="7"/>
       <c r="C4" s="3"/>
@@ -878,7 +1023,7 @@
       <c r="N4" s="8"/>
       <c r="P4" s="16"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="7"/>
       <c r="C5" s="3"/>
@@ -894,7 +1039,7 @@
       <c r="N5" s="8"/>
       <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="9" t="s">
         <v>31</v>
@@ -914,7 +1059,7 @@
       <c r="N6" s="8"/>
       <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3"/>
@@ -930,7 +1075,7 @@
       <c r="N7" s="8"/>
       <c r="P7" s="16"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="7" t="s">
         <v>30</v>
@@ -943,17 +1088,17 @@
         <v>44</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="25"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="22"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="7" t="s">
         <v>1</v>
@@ -964,19 +1109,19 @@
       <c r="F9" s="8"/>
       <c r="H9" s="16"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="21" t="s">
+      <c r="J9" s="19"/>
+      <c r="K9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="25" t="s">
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
@@ -989,15 +1134,15 @@
         <v>44</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="25"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="22"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="10" t="s">
         <v>2</v>
@@ -1008,17 +1153,17 @@
       <c r="F11" s="8"/>
       <c r="H11" s="16"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="25"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="22"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="3"/>
@@ -1027,17 +1172,20 @@
       <c r="F12" s="8"/>
       <c r="H12" s="16"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="25"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
+      <c r="S12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="3" t="s">
@@ -1050,17 +1198,23 @@
         <v>46</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="25"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="22"/>
+      <c r="S13" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="3" t="s">
@@ -1073,17 +1227,20 @@
         <v>47</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="25"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="22"/>
+      <c r="S14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="3" t="s">
@@ -1096,15 +1253,15 @@
         <v>49</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="25"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" s="19"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="22"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="3" t="s">
@@ -1117,15 +1274,15 @@
         <v>44</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="25"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1136,15 +1293,15 @@
       <c r="F17" s="8"/>
       <c r="H17" s="16"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="25"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1157,13 +1314,13 @@
       <c r="F18" s="8"/>
       <c r="H18" s="16"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="25"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="22"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1178,15 +1335,15 @@
         <v>46</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="25"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="22"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1197,15 +1354,15 @@
       <c r="F20" s="8"/>
       <c r="H20" s="16"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="25"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="22"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1218,15 +1375,15 @@
       <c r="F21" s="8"/>
       <c r="H21" s="16"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="25"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="22"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1239,15 +1396,15 @@
       <c r="F22" s="8"/>
       <c r="H22" s="16"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="25"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="22"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1262,13 +1419,13 @@
         <v>49</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="25"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="22"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1283,15 +1440,15 @@
         <v>46</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="25"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1302,15 +1459,15 @@
       <c r="F25" s="8"/>
       <c r="H25" s="16"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="25"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1323,15 +1480,15 @@
       <c r="F26" s="8"/>
       <c r="H26" s="16"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="25"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="22"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -1346,13 +1503,13 @@
         <v>48</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="31"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="28"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1363,15 +1520,15 @@
       <c r="F28" s="8"/>
       <c r="H28" s="16"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="27" t="s">
+      <c r="J28" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="25"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1384,15 +1541,15 @@
       <c r="F29" s="8"/>
       <c r="H29" s="16"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="25"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -1407,13 +1564,13 @@
         <v>46</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="25"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1424,15 +1581,15 @@
       <c r="F31" s="8"/>
       <c r="H31" s="16"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="25"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -1445,15 +1602,15 @@
       <c r="F32" s="8"/>
       <c r="H32" s="16"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="22" t="s">
+      <c r="J32" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="25"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="22"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
@@ -1468,13 +1625,13 @@
         <v>47</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="25"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="22"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -1489,15 +1646,15 @@
         <v>46</v>
       </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="22" t="s">
+      <c r="J34" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K34" s="32"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="25"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="22"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -1508,15 +1665,15 @@
       <c r="F35" s="8"/>
       <c r="H35" s="16"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="22" t="s">
+      <c r="J35" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="25"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="22"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -1529,15 +1686,15 @@
       <c r="F36" s="8"/>
       <c r="H36" s="16"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="22" t="s">
+      <c r="J36" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="25"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
@@ -1552,13 +1709,13 @@
         <v>47</v>
       </c>
       <c r="I37" s="3"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="25"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="22"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -1569,15 +1726,15 @@
       <c r="F38" s="8"/>
       <c r="H38" s="16"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="22" t="s">
+      <c r="J38" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="25"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="22"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -1590,15 +1747,15 @@
       <c r="F39" s="8"/>
       <c r="H39" s="16"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="22" t="s">
+      <c r="J39" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="25"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="22"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -1611,15 +1768,15 @@
       <c r="F40" s="8"/>
       <c r="H40" s="16"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="22" t="s">
+      <c r="J40" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="25"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="22"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -1911,4 +2068,342 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H21:H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="E5" s="42">
+        <v>42754</v>
+      </c>
+      <c r="F5" s="42">
+        <v>42755</v>
+      </c>
+      <c r="G5" s="42">
+        <v>42756</v>
+      </c>
+      <c r="H5" s="42">
+        <v>42757</v>
+      </c>
+      <c r="I5" s="42">
+        <v>42758</v>
+      </c>
+      <c r="J5" s="42">
+        <v>42759</v>
+      </c>
+      <c r="K5" s="42">
+        <v>42760</v>
+      </c>
+      <c r="L5" s="42">
+        <v>42761</v>
+      </c>
+      <c r="M5" s="42">
+        <v>42762</v>
+      </c>
+      <c r="N5" s="42">
+        <v>42763</v>
+      </c>
+      <c r="O5" s="42">
+        <v>42764</v>
+      </c>
+      <c r="P5" s="42">
+        <v>42765</v>
+      </c>
+      <c r="Q5" s="42">
+        <v>42766</v>
+      </c>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="C6" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>